<commit_message>
duchc: update Meeting minute.xlsx ngày 18/5/2015 tuần 2 ngày 1
</commit_message>
<xml_diff>
--- a/Source/Document/Meeting minutes/Meeting minute.xlsx
+++ b/Source/Document/Meeting minutes/Meeting minute.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="78">
   <si>
     <t>MEETING MINUTES</t>
   </si>
@@ -183,12 +183,6 @@
     <t>Sửa lại introduction rp1: giới thiệu chức năng của hệ thống</t>
   </si>
   <si>
-    <t>easy to use, reduce error: bỏ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Feature function: thiếu actor: system, thống kê doanh thu, tìm kiếm của khách hàng, system support payment, advance product search</t>
   </si>
   <si>
@@ -222,10 +216,43 @@
     <t>tracking sản phẩm, đưa sản phẩm lên đúng mùa</t>
   </si>
   <si>
-    <t>Chia lại task trong 6.functional requirement</t>
-  </si>
-  <si>
     <t>Vẽ core flow của ứng dụng. Làm prototype của core flow</t>
+  </si>
+  <si>
+    <t>Chia lại task trong 6.functional requirement của rp1</t>
+  </si>
+  <si>
+    <t>Sửa shop owner thành store owner</t>
+  </si>
+  <si>
+    <t>Phân biệt guest và customer</t>
+  </si>
+  <si>
+    <t>không dùng "easy to use" hay "reduce error". Chỉ viết những thứ làm được</t>
+  </si>
+  <si>
+    <t>Software Process Model trong rp2 chia lại điểm thành phần. Lưu ý: không ghi gì là max điểm, có lúc cả thành phần đều không đạt yêu cầu</t>
+  </si>
+  <si>
+    <t>Làm rõ phần bán hàng</t>
+  </si>
+  <si>
+    <t>Trong rp2 -&gt; Tool and Technique -&gt; Domain knowledge thêm consigment aspect</t>
+  </si>
+  <si>
+    <t>Coding convention: phần comment không nên ghi, những phần nào tuân thủ được thì để lại</t>
+  </si>
+  <si>
+    <t>duchc</t>
+  </si>
+  <si>
+    <t>danqt</t>
+  </si>
+  <si>
+    <t>phuctq</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dantq, hoangnh</t>
   </si>
 </sst>
 </file>
@@ -441,6 +468,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -449,9 +479,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -774,22 +801,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
@@ -798,20 +825,20 @@
       <c r="T1" s="4"/>
     </row>
     <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -820,20 +847,20 @@
       <c r="T2" s="4"/>
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -842,20 +869,20 @@
       <c r="T3" s="4"/>
     </row>
     <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
@@ -868,42 +895,42 @@
         <v>1</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="25" t="s">
+      <c r="D5" s="27"/>
+      <c r="E5" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="25" t="s">
+      <c r="F5" s="27"/>
+      <c r="G5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="26"/>
-      <c r="I5" s="25" t="s">
+      <c r="H5" s="27"/>
+      <c r="I5" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="26"/>
-      <c r="K5" s="25" t="s">
+      <c r="J5" s="27"/>
+      <c r="K5" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="26"/>
-      <c r="M5" s="25" t="s">
+      <c r="L5" s="27"/>
+      <c r="M5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="26"/>
-      <c r="O5" s="25" t="s">
+      <c r="N5" s="27"/>
+      <c r="O5" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="25" t="s">
+      <c r="P5" s="27"/>
+      <c r="Q5" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="R5" s="26"/>
-      <c r="S5" s="25" t="s">
+      <c r="R5" s="27"/>
+      <c r="S5" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="T5" s="26"/>
+      <c r="T5" s="27"/>
     </row>
     <row r="6" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -1277,8 +1304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B3" sqref="A1:C11"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1479,10 +1506,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1525,69 +1552,145 @@
         <v>2</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="39" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
         <v>3</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="17"/>
+        <v>69</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A6" s="16">
         <v>4</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="17"/>
+      <c r="B6" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
         <v>5</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="17"/>
-    </row>
-    <row r="8" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="B7" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="58.5" x14ac:dyDescent="0.3">
       <c r="A8" s="16">
         <v>6</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="17"/>
+      <c r="B8" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="39" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
         <v>7</v>
       </c>
-      <c r="B9" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="17"/>
+      <c r="B9" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
+      <c r="A10" s="16">
+        <v>8</v>
+      </c>
       <c r="B10" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="17"/>
+    </row>
+    <row r="11" spans="1:3" ht="39" x14ac:dyDescent="0.3">
+      <c r="A11" s="16">
+        <v>9</v>
+      </c>
+      <c r="B11" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="17"/>
-    </row>
-    <row r="11" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="16">
-        <v>7</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="17"/>
+      <c r="C11" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="16">
+        <v>10</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="39" x14ac:dyDescent="0.3">
+      <c r="A13" s="16">
+        <v>11</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="39" x14ac:dyDescent="0.3">
+      <c r="A14" s="16">
+        <v>12</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="17"/>
+    </row>
+    <row r="16" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="21"/>
+    </row>
+    <row r="17" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1603,39 +1706,39 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
         <v>57</v>
-      </c>
-      <c r="B1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
         <v>58</v>
-      </c>
-      <c r="B2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DucHC: update Meeting minute.xlsx 20/5/2015
</commit_message>
<xml_diff>
--- a/Source/Document/Meeting minutes/Meeting minute.xlsx
+++ b/Source/Document/Meeting minutes/Meeting minute.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,15 @@
     <sheet name="W1_2" sheetId="3" r:id="rId4"/>
     <sheet name="W2_1" sheetId="4" r:id="rId5"/>
     <sheet name="W2_2" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="103">
   <si>
     <t>MEETING MINUTES</t>
   </si>
@@ -283,13 +285,70 @@
   </si>
   <si>
     <t>Report 3</t>
+  </si>
+  <si>
+    <t>Store owner side: thiếu ngày tháng</t>
+  </si>
+  <si>
+    <t>Nên có màu sắc cho những hàng xác thực được</t>
+  </si>
+  <si>
+    <t>Canh những trạng thái đều nhau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Từ  status về sau nên bỏ đi vì ko phù hợp HCI - focus vào 1 chức năng mà ở đây là deal request. Khi check vào sp là đã đọc rồi. Khách hàng thường phải check sp trước khi mua, store owner cũng phải check xong mới lấy. </t>
+  </si>
+  <si>
+    <t>HCI sửa lại (thiết kế web, ko fải đt)</t>
+  </si>
+  <si>
+    <t>consign - đk món hàng -&gt; thông báo khách hàng -&gt; đồng ý thì điền thông tin cá nhân</t>
+  </si>
+  <si>
+    <t>Nếu món hàng phức tạp, thông khách hàng chờ vài ngày và chờ confirm, chọn store trước và cuối cùng confirm mới nhập thông tin cá nhân</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Home: panel thay thế bằng hàng hot, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hai bên hông dùng quảng cáo</t>
+    </r>
+  </si>
+  <si>
+    <t>thuật toán đưa hàng hot nhất chớp chớp ngay đầu</t>
+  </si>
+  <si>
+    <t>Payment: on web link tới product. Action có sold -&gt; chuyyển wa paypal thanh toán luôn. Các action khác chỉ link tới sp. Có set thời gian trả hàng. Trang chỉ nên có item name và ngày gửi</t>
+  </si>
+  <si>
+    <t>Phải có cơ chế offline và online</t>
+  </si>
+  <si>
+    <t>Add to cart: để trong details -&gt; bắt ng dùng đọc để tránh phiền phức sau này</t>
+  </si>
+  <si>
+    <t>khi vào trang, cung cấp nhiều thông tin nhất có thể, hạn chế làm cho ng dùng kéo xuống</t>
+  </si>
+  <si>
+    <t>hướng kết hợp category ngang và dọc, hướng tới tối ưu giao diện cho ng dùng vào xem</t>
+  </si>
+  <si>
+    <t>Tâm lý người dùng: bán hàng nhanh nhất và mua hàng nhanh nhất</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -351,8 +410,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,6 +440,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -432,7 +504,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -501,6 +573,21 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -510,20 +597,20 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -833,7 +920,7 @@
   <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,22 +933,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
@@ -870,20 +957,20 @@
       <c r="T1" s="4"/>
     </row>
     <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -892,20 +979,20 @@
       <c r="T2" s="4"/>
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -914,20 +1001,20 @@
       <c r="T3" s="4"/>
     </row>
     <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
@@ -940,42 +1027,42 @@
         <v>1</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="26" t="s">
+      <c r="D5" s="32"/>
+      <c r="E5" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="26" t="s">
+      <c r="F5" s="32"/>
+      <c r="G5" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="27"/>
-      <c r="I5" s="26" t="s">
+      <c r="H5" s="32"/>
+      <c r="I5" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="27"/>
-      <c r="K5" s="26" t="s">
+      <c r="J5" s="32"/>
+      <c r="K5" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="27"/>
-      <c r="M5" s="26" t="s">
+      <c r="L5" s="32"/>
+      <c r="M5" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="27"/>
-      <c r="O5" s="26" t="s">
+      <c r="N5" s="32"/>
+      <c r="O5" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="26" t="s">
+      <c r="P5" s="32"/>
+      <c r="Q5" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="R5" s="27"/>
-      <c r="S5" s="26" t="s">
+      <c r="R5" s="32"/>
+      <c r="S5" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="T5" s="27"/>
+      <c r="T5" s="32"/>
     </row>
     <row r="6" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -1051,7 +1138,9 @@
       <c r="E8" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1083,7 +1172,9 @@
       <c r="E9" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1113,7 +1204,9 @@
       <c r="E10" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1143,7 +1236,9 @@
       <c r="E11" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1173,7 +1268,9 @@
       <c r="E12" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1217,120 +1314,120 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" style="31" customWidth="1"/>
-    <col min="2" max="2" width="82" style="32" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="31"/>
+    <col min="1" max="1" width="28.7109375" style="28" customWidth="1"/>
+    <col min="2" max="2" width="82" style="29" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="30" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="26" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="26" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="26" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="26" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="28" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="29"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="26"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="29"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="26"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="29"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="26"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="29"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="26"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="29"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="26"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="28" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="B15" s="29"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="26"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="29"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="26"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="26"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="26"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="28" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="B21" s="29"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="26"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
-      <c r="B22" s="29"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="26"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
-      <c r="B23" s="29"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="26"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="B24" s="29"/>
+      <c r="A24" s="27"/>
+      <c r="B24" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1693,8 +1790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection sqref="A1:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1937,11 +2034,451 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="72.85546875" style="37" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="34"/>
+    </row>
+    <row r="2" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="16">
+        <v>1</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="17"/>
+    </row>
+    <row r="4" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="16">
+        <v>2</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="17"/>
+    </row>
+    <row r="5" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="16">
+        <v>3</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="17"/>
+    </row>
+    <row r="6" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="16">
+        <v>4</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="17"/>
+    </row>
+    <row r="7" spans="1:3" ht="78" x14ac:dyDescent="0.3">
+      <c r="A7" s="16">
+        <v>5</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="17"/>
+    </row>
+    <row r="8" spans="1:3" ht="39" x14ac:dyDescent="0.3">
+      <c r="A8" s="16">
+        <v>6</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="17"/>
+    </row>
+    <row r="9" spans="1:3" ht="58.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="16">
+        <v>7</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="17"/>
+    </row>
+    <row r="10" spans="1:3" ht="39" x14ac:dyDescent="0.3">
+      <c r="A10" s="16">
+        <v>8</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="17"/>
+    </row>
+    <row r="11" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="16">
+        <v>9</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="17"/>
+    </row>
+    <row r="12" spans="1:3" ht="78" x14ac:dyDescent="0.3">
+      <c r="A12" s="16">
+        <v>10</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="17"/>
+    </row>
+    <row r="13" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="16">
+        <v>11</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="17"/>
+    </row>
+    <row r="14" spans="1:3" ht="39" x14ac:dyDescent="0.3">
+      <c r="A14" s="16">
+        <v>12</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="17"/>
+    </row>
+    <row r="15" spans="1:3" ht="39" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="17"/>
+    </row>
+    <row r="16" spans="1:3" ht="39" x14ac:dyDescent="0.3">
+      <c r="A16" s="16"/>
+      <c r="B16" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="17"/>
+    </row>
+    <row r="17" spans="1:3" ht="39" x14ac:dyDescent="0.3">
+      <c r="A17" s="16"/>
+      <c r="B17" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="17"/>
+    </row>
+    <row r="18" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="16"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="17"/>
+    </row>
+    <row r="19" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="16"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="17"/>
+    </row>
+    <row r="20" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="16"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="17"/>
+    </row>
+    <row r="21" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A21" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="34"/>
+    </row>
+    <row r="22" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A23" s="17"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="17"/>
+    </row>
+    <row r="24" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="17"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="17"/>
+    </row>
+    <row r="25" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="17"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="17"/>
+    </row>
+    <row r="26" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A26" s="17"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="17"/>
+    </row>
+    <row r="27" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A27" s="17"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="17"/>
+    </row>
+    <row r="28" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A28" s="17"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="17"/>
+    </row>
+    <row r="29" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A29" s="17"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="17"/>
+    </row>
+    <row r="30" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A30" s="17"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="17"/>
+    </row>
+    <row r="31" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A31" s="17"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="17"/>
+    </row>
+    <row r="32" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A32" s="17"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="34"/>
+    </row>
+    <row r="2" spans="1:3" ht="39" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="16">
+        <v>1</v>
+      </c>
+      <c r="B3" s="26"/>
+      <c r="C3" s="17"/>
+    </row>
+    <row r="4" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="16">
+        <v>2</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="17"/>
+    </row>
+    <row r="5" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="16">
+        <v>3</v>
+      </c>
+      <c r="B5" s="26"/>
+      <c r="C5" s="17"/>
+    </row>
+    <row r="6" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="16">
+        <v>4</v>
+      </c>
+      <c r="B6" s="26"/>
+      <c r="C6" s="17"/>
+    </row>
+    <row r="7" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="16">
+        <v>5</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" s="17"/>
+    </row>
+    <row r="8" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="16">
+        <v>6</v>
+      </c>
+      <c r="B8" s="26"/>
+      <c r="C8" s="17"/>
+    </row>
+    <row r="9" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="16">
+        <v>7</v>
+      </c>
+      <c r="B9" s="36"/>
+      <c r="C9" s="17"/>
+    </row>
+    <row r="10" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="16">
+        <v>8</v>
+      </c>
+      <c r="B10" s="26"/>
+      <c r="C10" s="17"/>
+    </row>
+    <row r="11" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="16">
+        <v>9</v>
+      </c>
+      <c r="B11" s="26"/>
+      <c r="C11" s="17"/>
+    </row>
+    <row r="12" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="16">
+        <v>10</v>
+      </c>
+      <c r="B12" s="26"/>
+      <c r="C12" s="17"/>
+    </row>
+    <row r="13" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="16">
+        <v>11</v>
+      </c>
+      <c r="B13" s="26"/>
+      <c r="C13" s="17"/>
+    </row>
+    <row r="14" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="16">
+        <v>12</v>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="17"/>
+    </row>
+    <row r="15" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="17"/>
+    </row>
+    <row r="16" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="34"/>
+    </row>
+    <row r="17" spans="1:3" ht="39" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="17"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="17"/>
+    </row>
+    <row r="19" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="17"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="17"/>
+    </row>
+    <row r="20" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="17"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="17"/>
+    </row>
+    <row r="21" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="17"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="17"/>
+    </row>
+    <row r="22" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A22" s="17"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="17"/>
+    </row>
+    <row r="23" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A23" s="17"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="17"/>
+    </row>
+    <row r="24" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="17"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="17"/>
+    </row>
+    <row r="25" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="17"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="17"/>
+    </row>
+    <row r="26" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A26" s="17"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="17"/>
+    </row>
+    <row r="27" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A27" s="17"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Duchc: commit Meeting minute.xlsx 25/5
</commit_message>
<xml_diff>
--- a/Source/Document/Meeting minutes/Meeting minute.xlsx
+++ b/Source/Document/Meeting minutes/Meeting minute.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="W1_2" sheetId="3" r:id="rId4"/>
     <sheet name="W2_1" sheetId="4" r:id="rId5"/>
     <sheet name="W2_2" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="8" r:id="rId7"/>
+    <sheet name="W3_1" sheetId="8" r:id="rId7"/>
     <sheet name="Sheet2" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="120">
   <si>
     <t>MEETING MINUTES</t>
   </si>
@@ -342,6 +342,57 @@
   </si>
   <si>
     <t>Tâm lý người dùng: bán hàng nhanh nhất và mua hàng nhanh nhất</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sửa lại css, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khảo sát </t>
+  </si>
+  <si>
+    <t>Cửa hàng thêm giá riêng và độ tin cậy</t>
+  </si>
+  <si>
+    <t>Cho thêm Category lúc chọn sp và và xét category mà store muốn mua</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Không cung cấp CMND</t>
+  </si>
+  <si>
+    <t>Chọn email làm phương thức liên lạc chính, phone chỉ là option</t>
+  </si>
+  <si>
+    <t>Trang web làm ra để khách hàng cần mình</t>
+  </si>
+  <si>
+    <t>Address cũng không cần phải điền</t>
+  </si>
+  <si>
+    <t>Liên lạc phải verify đc mới có giá trị</t>
+  </si>
+  <si>
+    <t>Credit card ko cần điền, cho phép tới cửa hàng lấy tiền</t>
+  </si>
+  <si>
+    <t>Credit card phải thêm thông tin cửa người thụ hưởng</t>
+  </si>
+  <si>
+    <t>Màu sắc phải có màu chủ đạo, ko dùng nhiều màu</t>
+  </si>
+  <si>
+    <t>Use case phải là 2.0</t>
+  </si>
+  <si>
+    <t>Tên use case phải chính xác</t>
+  </si>
+  <si>
+    <t>Thêm new feed cho store owner</t>
+  </si>
+  <si>
+    <t>Bỏ hình ảnh trong list</t>
+  </si>
+  <si>
+    <t>Bỏ cột verify min price, max price</t>
   </si>
 </sst>
 </file>
@@ -504,7 +555,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -588,6 +639,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -596,21 +659,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -933,22 +981,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
@@ -957,20 +1005,20 @@
       <c r="T1" s="4"/>
     </row>
     <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -979,20 +1027,20 @@
       <c r="T2" s="4"/>
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -1001,20 +1049,20 @@
       <c r="T3" s="4"/>
     </row>
     <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
@@ -1027,42 +1075,42 @@
         <v>1</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="31" t="s">
+      <c r="D5" s="36"/>
+      <c r="E5" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="32"/>
-      <c r="G5" s="31" t="s">
+      <c r="F5" s="36"/>
+      <c r="G5" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="32"/>
-      <c r="I5" s="31" t="s">
+      <c r="H5" s="36"/>
+      <c r="I5" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="32"/>
-      <c r="K5" s="31" t="s">
+      <c r="J5" s="36"/>
+      <c r="K5" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="32"/>
-      <c r="M5" s="31" t="s">
+      <c r="L5" s="36"/>
+      <c r="M5" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="32"/>
-      <c r="O5" s="31" t="s">
+      <c r="N5" s="36"/>
+      <c r="O5" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="31" t="s">
+      <c r="P5" s="36"/>
+      <c r="Q5" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="R5" s="32"/>
-      <c r="S5" s="31" t="s">
+      <c r="R5" s="36"/>
+      <c r="S5" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="T5" s="32"/>
+      <c r="T5" s="36"/>
     </row>
     <row r="6" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -2036,14 +2084,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="72.85546875" style="37" customWidth="1"/>
+    <col min="2" max="2" width="72.85546875" style="33" customWidth="1"/>
     <col min="3" max="3" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2051,13 +2099,13 @@
       <c r="A1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="32" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -2122,7 +2170,7 @@
       <c r="A9" s="16">
         <v>7</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="34" t="s">
         <v>94</v>
       </c>
       <c r="C9" s="17"/>
@@ -2212,13 +2260,13 @@
       <c r="A21" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="34"/>
+      <c r="B21" s="31"/>
     </row>
     <row r="22" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="32" t="s">
         <v>24</v>
       </c>
       <c r="C22" s="15" t="s">
@@ -2283,10 +2331,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2300,13 +2348,13 @@
       <c r="A1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="34"/>
+      <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:3" ht="39" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="32" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -2317,137 +2365,177 @@
       <c r="A3" s="16">
         <v>1</v>
       </c>
-      <c r="B3" s="26"/>
+      <c r="B3" s="26" t="s">
+        <v>103</v>
+      </c>
       <c r="C3" s="17"/>
     </row>
     <row r="4" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A4" s="16">
         <v>2</v>
       </c>
-      <c r="B4" s="26"/>
+      <c r="B4" s="26" t="s">
+        <v>104</v>
+      </c>
       <c r="C4" s="17"/>
     </row>
     <row r="5" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
         <v>3</v>
       </c>
-      <c r="B5" s="26"/>
+      <c r="B5" s="26" t="s">
+        <v>105</v>
+      </c>
       <c r="C5" s="17"/>
     </row>
-    <row r="6" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="39" x14ac:dyDescent="0.3">
       <c r="A6" s="16">
         <v>4</v>
       </c>
-      <c r="B6" s="26"/>
+      <c r="B6" s="26" t="s">
+        <v>106</v>
+      </c>
       <c r="C6" s="17"/>
     </row>
     <row r="7" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
         <v>5</v>
       </c>
-      <c r="B7" s="26"/>
+      <c r="B7" s="26" t="s">
+        <v>107</v>
+      </c>
       <c r="C7" s="17"/>
     </row>
-    <row r="8" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="39" x14ac:dyDescent="0.3">
       <c r="A8" s="16">
         <v>6</v>
       </c>
-      <c r="B8" s="26"/>
+      <c r="B8" s="26" t="s">
+        <v>108</v>
+      </c>
       <c r="C8" s="17"/>
     </row>
     <row r="9" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
         <v>7</v>
       </c>
-      <c r="B9" s="36"/>
+      <c r="B9" s="34" t="s">
+        <v>109</v>
+      </c>
       <c r="C9" s="17"/>
     </row>
     <row r="10" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A10" s="16">
         <v>8</v>
       </c>
-      <c r="B10" s="26"/>
+      <c r="B10" s="26" t="s">
+        <v>110</v>
+      </c>
       <c r="C10" s="17"/>
     </row>
     <row r="11" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A11" s="16">
         <v>9</v>
       </c>
-      <c r="B11" s="26"/>
+      <c r="B11" s="26" t="s">
+        <v>111</v>
+      </c>
       <c r="C11" s="17"/>
     </row>
-    <row r="12" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="39" x14ac:dyDescent="0.3">
       <c r="A12" s="16">
         <v>10</v>
       </c>
-      <c r="B12" s="26"/>
+      <c r="B12" s="26" t="s">
+        <v>112</v>
+      </c>
       <c r="C12" s="17"/>
     </row>
-    <row r="13" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="39" x14ac:dyDescent="0.3">
       <c r="A13" s="16">
         <v>11</v>
       </c>
-      <c r="B13" s="26"/>
+      <c r="B13" s="26" t="s">
+        <v>113</v>
+      </c>
       <c r="C13" s="17"/>
     </row>
     <row r="14" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A14" s="16">
         <v>12</v>
       </c>
-      <c r="B14" s="26"/>
+      <c r="B14" s="26" t="s">
+        <v>114</v>
+      </c>
       <c r="C14" s="17"/>
     </row>
     <row r="15" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
+      <c r="A15" s="16">
+        <v>13</v>
+      </c>
       <c r="B15" s="26"/>
       <c r="C15" s="17"/>
     </row>
-    <row r="16" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A16" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="34"/>
-    </row>
-    <row r="17" spans="1:3" ht="39" x14ac:dyDescent="0.3">
-      <c r="A17" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>29</v>
-      </c>
+    <row r="16" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="17"/>
+    </row>
+    <row r="17" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="16">
+        <v>15</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="17"/>
     </row>
     <row r="18" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="26" t="s">
+        <v>117</v>
+      </c>
       <c r="C18" s="17"/>
     </row>
     <row r="19" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="26" t="s">
+        <v>118</v>
+      </c>
       <c r="C19" s="17"/>
     </row>
     <row r="20" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="26"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="26" t="s">
+        <v>119</v>
+      </c>
       <c r="C20" s="17"/>
     </row>
     <row r="21" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="26"/>
       <c r="C21" s="17"/>
     </row>
-    <row r="22" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="17"/>
-    </row>
-    <row r="23" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="17"/>
+    <row r="22" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A22" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="31"/>
+    </row>
+    <row r="23" spans="1:3" ht="39" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="24" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A24" s="17"/>
@@ -2468,6 +2556,36 @@
       <c r="A27" s="17"/>
       <c r="B27" s="26"/>
       <c r="C27" s="17"/>
+    </row>
+    <row r="28" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A28" s="17"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="17"/>
+    </row>
+    <row r="29" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A29" s="17"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="17"/>
+    </row>
+    <row r="30" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A30" s="17"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="17"/>
+    </row>
+    <row r="31" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A31" s="17"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="17"/>
+    </row>
+    <row r="32" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A32" s="17"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="17"/>
+    </row>
+    <row r="33" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A33" s="17"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
DucHC: update Meeting minute.xlsx
</commit_message>
<xml_diff>
--- a/Source/Document/Meeting minutes/Meeting minute.xlsx
+++ b/Source/Document/Meeting minutes/Meeting minute.xlsx
@@ -14,14 +14,14 @@
     <sheet name="W2_1" sheetId="4" r:id="rId5"/>
     <sheet name="W2_2" sheetId="6" r:id="rId6"/>
     <sheet name="W3_1" sheetId="8" r:id="rId7"/>
-    <sheet name="Sheet2" sheetId="9" r:id="rId8"/>
+    <sheet name="W3_2" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="125">
   <si>
     <t>MEETING MINUTES</t>
   </si>
@@ -350,18 +350,9 @@
     <t xml:space="preserve">Khảo sát </t>
   </si>
   <si>
-    <t>Cửa hàng thêm giá riêng và độ tin cậy</t>
-  </si>
-  <si>
-    <t>Cho thêm Category lúc chọn sp và và xét category mà store muốn mua</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Không cung cấp CMND</t>
   </si>
   <si>
-    <t>Chọn email làm phương thức liên lạc chính, phone chỉ là option</t>
-  </si>
-  <si>
     <t>Trang web làm ra để khách hàng cần mình</t>
   </si>
   <si>
@@ -393,6 +384,30 @@
   </si>
   <si>
     <t>Bỏ cột verify min price, max price</t>
+  </si>
+  <si>
+    <t>Bữa sau nếu sai nhóm trưởng bị trừ điểm</t>
+  </si>
+  <si>
+    <t>Sửa lại usecase diagram</t>
+  </si>
+  <si>
+    <t>extent khi thỏa đk nào đó mới thực hiện</t>
+  </si>
+  <si>
+    <t>Chọn email làm phương thức liên lạc chính, phone chỉ là option hoặc do ng dùng lựa chọn</t>
+  </si>
+  <si>
+    <t>Chọn cửa hàng thêm giá riêng và độ tin cậy</t>
+  </si>
+  <si>
+    <t>Cho thêm Category lúc điền thông tin sp và và xét category mà store muốn mua</t>
+  </si>
+  <si>
+    <t>25/5/2015</t>
+  </si>
+  <si>
+    <t>27/5/2015</t>
   </si>
 </sst>
 </file>
@@ -555,7 +570,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -659,6 +674,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -968,7 +995,7 @@
   <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,8 +1156,12 @@
       <c r="F6" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
+      <c r="G6" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>124</v>
+      </c>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
@@ -1156,7 +1187,9 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1">
+        <v>105</v>
+      </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -1189,8 +1222,12 @@
       <c r="F8" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -1223,8 +1260,12 @@
       <c r="F9" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1255,8 +1296,12 @@
       <c r="F10" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -1287,8 +1332,12 @@
       <c r="F11" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1319,8 +1368,12 @@
       <c r="F12" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -1352,6 +1405,8 @@
     <hyperlink ref="D6" location="W1_2!A1" display="13/5/2015"/>
     <hyperlink ref="E6" location="W2_1!A1" display="18/5/2015"/>
     <hyperlink ref="F6" location="W2_2!A1" display="20/5/2015"/>
+    <hyperlink ref="G6" location="W3_1!A1" display="25/5/2015"/>
+    <hyperlink ref="H6" location="W3_2!A1" display="27/5/2015"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2331,10 +2386,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2384,7 +2439,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="C5" s="17"/>
     </row>
@@ -2393,7 +2448,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="C6" s="17"/>
     </row>
@@ -2402,7 +2457,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C7" s="17"/>
     </row>
@@ -2411,7 +2466,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="C8" s="17"/>
     </row>
@@ -2420,7 +2475,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C9" s="17"/>
     </row>
@@ -2429,7 +2484,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C10" s="17"/>
     </row>
@@ -2438,7 +2493,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C11" s="17"/>
     </row>
@@ -2447,7 +2502,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C12" s="17"/>
     </row>
@@ -2456,7 +2511,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C13" s="17"/>
     </row>
@@ -2465,7 +2520,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C14" s="17"/>
     </row>
@@ -2473,7 +2528,9 @@
       <c r="A15" s="16">
         <v>13</v>
       </c>
-      <c r="B15" s="26"/>
+      <c r="B15" s="26" t="s">
+        <v>112</v>
+      </c>
       <c r="C15" s="17"/>
     </row>
     <row r="16" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
@@ -2481,7 +2538,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C16" s="17"/>
     </row>
@@ -2490,52 +2547,54 @@
         <v>15</v>
       </c>
       <c r="B17" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" s="17"/>
+    </row>
+    <row r="18" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="16">
+        <v>16</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18" s="17"/>
+    </row>
+    <row r="19" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="16">
+        <v>17</v>
+      </c>
+      <c r="B19" s="26" t="s">
         <v>116</v>
-      </c>
-      <c r="C17" s="17"/>
-    </row>
-    <row r="18" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="16"/>
-      <c r="B18" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="C18" s="17"/>
-    </row>
-    <row r="19" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="16"/>
-      <c r="B19" s="26" t="s">
-        <v>118</v>
       </c>
       <c r="C19" s="17"/>
     </row>
     <row r="20" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A20" s="16"/>
-      <c r="B20" s="26" t="s">
-        <v>119</v>
-      </c>
+      <c r="B20" s="26"/>
       <c r="C20" s="17"/>
     </row>
-    <row r="21" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="16"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="17"/>
-    </row>
-    <row r="22" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A22" s="12" t="s">
+    <row r="21" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A21" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="31"/>
-    </row>
-    <row r="23" spans="1:3" ht="39" x14ac:dyDescent="0.3">
-      <c r="A23" s="18" t="s">
+      <c r="B21" s="31"/>
+    </row>
+    <row r="22" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="32" t="s">
+      <c r="B22" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C22" s="15" t="s">
         <v>29</v>
       </c>
+    </row>
+    <row r="23" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A23" s="17"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="17"/>
     </row>
     <row r="24" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A24" s="17"/>
@@ -2581,11 +2640,6 @@
       <c r="A32" s="17"/>
       <c r="B32" s="26"/>
       <c r="C32" s="17"/>
-    </row>
-    <row r="33" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A33" s="17"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2594,12 +2648,235 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55" style="13" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="38"/>
+    </row>
+    <row r="2" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="16">
+        <v>1</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="17"/>
+    </row>
+    <row r="4" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="16">
+        <v>2</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="17"/>
+    </row>
+    <row r="5" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="16">
+        <v>3</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="17"/>
+    </row>
+    <row r="6" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="16">
+        <v>4</v>
+      </c>
+      <c r="B6" s="40"/>
+      <c r="C6" s="17"/>
+    </row>
+    <row r="7" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="16">
+        <v>5</v>
+      </c>
+      <c r="B7" s="40"/>
+      <c r="C7" s="17"/>
+    </row>
+    <row r="8" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="16">
+        <v>6</v>
+      </c>
+      <c r="B8" s="40"/>
+      <c r="C8" s="17"/>
+    </row>
+    <row r="9" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="16">
+        <v>7</v>
+      </c>
+      <c r="B9" s="41"/>
+      <c r="C9" s="17"/>
+    </row>
+    <row r="10" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="16">
+        <v>8</v>
+      </c>
+      <c r="B10" s="40"/>
+      <c r="C10" s="17"/>
+    </row>
+    <row r="11" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="16">
+        <v>9</v>
+      </c>
+      <c r="B11" s="40"/>
+      <c r="C11" s="17"/>
+    </row>
+    <row r="12" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="16">
+        <v>10</v>
+      </c>
+      <c r="B12" s="40"/>
+      <c r="C12" s="17"/>
+    </row>
+    <row r="13" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="16">
+        <v>11</v>
+      </c>
+      <c r="B13" s="40"/>
+      <c r="C13" s="17"/>
+    </row>
+    <row r="14" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="16">
+        <v>12</v>
+      </c>
+      <c r="B14" s="40"/>
+      <c r="C14" s="17"/>
+    </row>
+    <row r="15" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="16">
+        <v>13</v>
+      </c>
+      <c r="B15" s="40"/>
+      <c r="C15" s="17"/>
+    </row>
+    <row r="16" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="16">
+        <v>14</v>
+      </c>
+      <c r="B16" s="40"/>
+      <c r="C16" s="17"/>
+    </row>
+    <row r="17" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="16">
+        <v>15</v>
+      </c>
+      <c r="B17" s="40"/>
+      <c r="C17" s="17"/>
+    </row>
+    <row r="18" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="16"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="17"/>
+    </row>
+    <row r="19" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="16"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="17"/>
+    </row>
+    <row r="20" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="16"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="17"/>
+    </row>
+    <row r="21" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="16"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="17"/>
+    </row>
+    <row r="22" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A22" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="38"/>
+    </row>
+    <row r="23" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="17"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="17"/>
+    </row>
+    <row r="25" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="17"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="17"/>
+    </row>
+    <row r="26" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A26" s="17"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="17"/>
+    </row>
+    <row r="27" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A27" s="17"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="17"/>
+    </row>
+    <row r="28" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A28" s="17"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="17"/>
+    </row>
+    <row r="29" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A29" s="17"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="17"/>
+    </row>
+    <row r="30" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A30" s="17"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="17"/>
+    </row>
+    <row r="31" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A31" s="17"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="17"/>
+    </row>
+    <row r="32" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A32" s="17"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="17"/>
+    </row>
+    <row r="33" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A33" s="17"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="17"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update: Capstone Project Document.docx Meeting minute.xlsx
</commit_message>
<xml_diff>
--- a/Source/Document/Meeting minutes/Meeting minute.xlsx
+++ b/Source/Document/Meeting minutes/Meeting minute.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="175">
   <si>
     <t>MEETING MINUTES</t>
   </si>
@@ -572,6 +572,12 @@
   </si>
   <si>
     <t>Định Policy cho bán đồ cũ, trả tiền trực tiếp</t>
+  </si>
+  <si>
+    <t>Phuc</t>
+  </si>
+  <si>
+    <t>Hoang</t>
   </si>
 </sst>
 </file>
@@ -1196,8 +1202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,7 +1212,9 @@
     <col min="2" max="2" width="10.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="3"/>
+    <col min="5" max="11" width="9.140625" style="3"/>
+    <col min="12" max="12" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1430,8 +1438,12 @@
       <c r="J6" s="6">
         <v>42069</v>
       </c>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
+      <c r="K6" s="6">
+        <v>42222</v>
+      </c>
+      <c r="L6" s="6">
+        <v>42283</v>
+      </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="8"/>
@@ -1780,6 +1792,8 @@
     <hyperlink ref="H6" location="W3_2!A1" display="27/5/2015"/>
     <hyperlink ref="I6" location="W4_1!A1" display="1/6/2015"/>
     <hyperlink ref="J6" location="W4_2!A1" display="3/6/2015"/>
+    <hyperlink ref="K6" location="W5_1!A1" display="8/6/2015"/>
+    <hyperlink ref="L6" location="W5_2!A1" display="10/6/2015"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2047,8 +2061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2083,7 +2097,9 @@
       <c r="B3" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="C3" s="26"/>
+      <c r="C3" s="26" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A4" s="41">
@@ -2092,7 +2108,9 @@
       <c r="B4" s="36" t="s">
         <v>167</v>
       </c>
-      <c r="C4" s="26"/>
+      <c r="C4" s="26" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A5" s="41">
@@ -2101,7 +2119,9 @@
       <c r="B5" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="C5" s="26"/>
+      <c r="C5" s="26" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A6" s="41">
@@ -2110,7 +2130,9 @@
       <c r="B6" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="C6" s="26"/>
+      <c r="C6" s="26" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A7" s="41">
@@ -2128,7 +2150,9 @@
       <c r="B8" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="C8" s="26"/>
+      <c r="C8" s="26" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A9" s="41">

</xml_diff>

<commit_message>
Update: Meeting minute.xlsx consignment_request_receive.jsp manageProductStatusPage.jsp
</commit_message>
<xml_diff>
--- a/Source/Document/Meeting minutes/Meeting minute.xlsx
+++ b/Source/Document/Meeting minutes/Meeting minute.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="204">
   <si>
     <t>MEETING MINUTES</t>
   </si>
@@ -629,6 +629,48 @@
   </si>
   <si>
     <t>17/6/2015</t>
+  </si>
+  <si>
+    <t>30/6/2015</t>
+  </si>
+  <si>
+    <t>hub</t>
+  </si>
+  <si>
+    <t>ngay giao hang +1 +3 today</t>
+  </si>
+  <si>
+    <t>sp tra ve tren 10sp</t>
+  </si>
+  <si>
+    <t>gia se duoc dinh tai thoi diem nhan hang</t>
+  </si>
+  <si>
+    <t>radio button chon roi` next</t>
+  </si>
+  <si>
+    <t>ghi product name, brand auto fill</t>
+  </si>
+  <si>
+    <t>onclose()</t>
+  </si>
+  <si>
+    <t>onload()</t>
+  </si>
+  <si>
+    <t>hoa don ki gui</t>
+  </si>
+  <si>
+    <t>tien tra khach hang phai tinh san</t>
+  </si>
+  <si>
+    <t>2 ngay sau tra max tien</t>
+  </si>
+  <si>
+    <t>***</t>
+  </si>
+  <si>
+    <t>----</t>
   </si>
 </sst>
 </file>
@@ -808,7 +850,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -945,6 +987,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1253,8 +1298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1501,7 +1546,9 @@
       <c r="N6" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="O6" s="8"/>
+      <c r="O6" s="8" t="s">
+        <v>190</v>
+      </c>
       <c r="P6" s="8"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
@@ -1597,7 +1644,9 @@
       <c r="N8" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="O8" s="1"/>
+      <c r="O8" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
@@ -1655,7 +1704,9 @@
       <c r="N9" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="O9" s="1"/>
+      <c r="O9" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -1763,7 +1814,9 @@
       <c r="N11" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="O11" s="1"/>
+      <c r="O11" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
@@ -1819,7 +1872,9 @@
       <c r="N12" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="O12" s="1"/>
+      <c r="O12" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
@@ -3115,10 +3170,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3129,13 +3184,13 @@
     <col min="4" max="16384" width="9.140625" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="34"/>
     </row>
-    <row r="2" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>23</v>
       </c>
@@ -3146,98 +3201,126 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A3" s="41">
         <v>1</v>
       </c>
-      <c r="B3" s="36"/>
+      <c r="B3" s="36" t="s">
+        <v>191</v>
+      </c>
       <c r="C3" s="26"/>
-    </row>
-    <row r="4" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F3" s="32" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A4" s="41">
         <v>2</v>
       </c>
-      <c r="B4" s="36"/>
+      <c r="B4" s="36" t="s">
+        <v>192</v>
+      </c>
       <c r="C4" s="26"/>
-    </row>
-    <row r="5" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="F4" s="32" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A5" s="41">
         <v>3</v>
       </c>
-      <c r="B5" s="36"/>
+      <c r="B5" s="36" t="s">
+        <v>193</v>
+      </c>
       <c r="C5" s="26"/>
     </row>
-    <row r="6" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A6" s="41">
         <v>4</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="36" t="s">
+        <v>194</v>
+      </c>
       <c r="C6" s="26"/>
     </row>
-    <row r="7" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A7" s="41">
         <v>5</v>
       </c>
-      <c r="B7" s="36"/>
+      <c r="B7" s="36" t="s">
+        <v>195</v>
+      </c>
       <c r="C7" s="26"/>
     </row>
-    <row r="8" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A8" s="41">
         <v>6</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="26"/>
-    </row>
-    <row r="9" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="B8" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A9" s="41">
         <v>7</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="26"/>
-    </row>
-    <row r="10" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="37" t="s">
+        <v>199</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A10" s="41">
         <v>8</v>
       </c>
-      <c r="B10" s="36"/>
+      <c r="B10" s="36" t="s">
+        <v>200</v>
+      </c>
       <c r="C10" s="26"/>
     </row>
-    <row r="11" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A11" s="41">
         <v>9</v>
       </c>
-      <c r="B11" s="36"/>
+      <c r="B11" s="36" t="s">
+        <v>201</v>
+      </c>
       <c r="C11" s="26"/>
     </row>
-    <row r="12" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A12" s="41">
         <v>10</v>
       </c>
       <c r="B12" s="36"/>
       <c r="C12" s="26"/>
     </row>
-    <row r="13" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A13" s="41">
         <v>11</v>
       </c>
       <c r="B13" s="36"/>
       <c r="C13" s="26"/>
     </row>
-    <row r="14" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A14" s="41">
         <v>12</v>
       </c>
       <c r="B14" s="36"/>
       <c r="C14" s="26"/>
     </row>
-    <row r="15" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A15" s="41">
         <v>13</v>
       </c>
       <c r="B15" s="36"/>
       <c r="C15" s="26"/>
     </row>
-    <row r="16" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A16" s="41">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Meeting minute.xlsx Report - Chotot.docx
</commit_message>
<xml_diff>
--- a/Source/Document/Meeting minutes/Meeting minute.xlsx
+++ b/Source/Document/Meeting minutes/Meeting minute.xlsx
@@ -917,9 +917,6 @@
     <t>tìm hợp đồng dân sự</t>
   </si>
   <si>
-    <t>trên web yêu cầu đã duyệt sẽ chia 2 tab, tab tới cty dua hang va tab nvien di lay hang</t>
-  </si>
-  <si>
     <t xml:space="preserve">Khi nao tien den tay </t>
   </si>
   <si>
@@ -935,9 +932,6 @@
     <t>loi nhuan và doanh thu khác nhau phải tách biệt</t>
   </si>
   <si>
-    <t>Không cần phải chi tiết từng món hàng mà cần</t>
-  </si>
-  <si>
     <t>javascript_neu ko co hinh thi hien no image</t>
   </si>
   <si>
@@ -945,6 +939,12 @@
   </si>
   <si>
     <t>So sanh HPS Cam do. Hợp đồng dân sự</t>
+  </si>
+  <si>
+    <t>trên web yêu cầu đã duyệt có tới cty dua hang va tab nvien di lay hang</t>
+  </si>
+  <si>
+    <t>Không cần phải chi tiết từng món hàng</t>
   </si>
 </sst>
 </file>
@@ -5703,7 +5703,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5754,7 +5754,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="C5" s="26"/>
     </row>
@@ -5763,7 +5763,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C6" s="26"/>
     </row>
@@ -5772,7 +5772,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C7" s="26"/>
     </row>
@@ -5781,7 +5781,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C8" s="26"/>
     </row>
@@ -5790,7 +5790,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C9" s="26"/>
     </row>
@@ -5799,7 +5799,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C10" s="26"/>
     </row>
@@ -5808,7 +5808,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C11" s="26"/>
     </row>
@@ -5817,7 +5817,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C12" s="26"/>
     </row>
@@ -5826,7 +5826,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C13" s="26"/>
     </row>
@@ -5835,7 +5835,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C14" s="26"/>
     </row>

</xml_diff>

<commit_message>
Update advices for Project and Meeting minute.xlsx
</commit_message>
<xml_diff>
--- a/Source/Document/Meeting minutes/Meeting minute.xlsx
+++ b/Source/Document/Meeting minutes/Meeting minute.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="17" activeTab="25"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="18" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="307">
   <si>
     <t>MEETING MINUTES</t>
   </si>
@@ -990,6 +990,116 @@
   </si>
   <si>
     <t>Sửa: Sản phẩm đã đặt và đã bán</t>
+  </si>
+  <si>
+    <r>
+      <t>Dùng "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>chúng tôi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" khi thuyết trình</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Thuyết trình toàn bộ bằng </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tiếng Việt</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chạy demo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KHÔNG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dùng Cốc Cốc, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">NÊN </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sử dụng bằng ẩn danh hoặc trình duyệt khác. Dùng nhiều trình duyệt và giới thiệu rõ màn hình này là thuộc role nào</t>
+    </r>
+  </si>
+  <si>
+    <t>Không nói "để về em xem xét" -&gt; dùng "tôi đã sai", "tôi chưa làm nghĩ tới trường hợp đó", "nhóm tôi chưa làm chức năng này, nhưng nếu làm như thế chúng tôi sẽ làm thế này..."</t>
+  </si>
+  <si>
+    <t>Nếu câu hỏi khó và dài, phải hỏi lại câu hỏi rõ ràng mới trả lời -&gt; kéo thời gian và làm rõ câu hỏi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hoàng </t>
+  </si>
+  <si>
+    <t>Làm Cookie (có session) cho khách ký gửi</t>
+  </si>
+  <si>
+    <t>INTRODUCTION -&gt;  PROBLEM -&gt; SOLUTION (DATA SOURCE) -&gt; SCENARIOR (PREPARE- SEARCH ROUTE -&gt; ALGORITHM) -&gt; DEFINATION -&gt; SUMMARY-&gt; FUTURE PLAN</t>
+  </si>
+  <si>
+    <t>SLIDE: Mình làm mọi thứ bằg tay NHƯ THẾ NÀO? Trả lời câu hỏi: "HOW"</t>
+  </si>
+  <si>
+    <t>Không nói công nghệ sử dụng.</t>
   </si>
 </sst>
 </file>
@@ -5762,14 +5872,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" style="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64" style="32" customWidth="1"/>
+    <col min="2" max="2" width="91.7109375" style="32" customWidth="1"/>
     <col min="3" max="3" width="27.42578125" style="32" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="32"/>
   </cols>
@@ -5903,7 +6013,9 @@
       <c r="A15" s="41">
         <v>13</v>
       </c>
-      <c r="B15" s="36"/>
+      <c r="B15" s="36" t="s">
+        <v>303</v>
+      </c>
       <c r="C15" s="26"/>
     </row>
     <row r="16" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
@@ -5913,21 +6025,27 @@
       <c r="B16" s="36"/>
       <c r="C16" s="26"/>
     </row>
-    <row r="17" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="58.5" x14ac:dyDescent="0.25">
       <c r="A17" s="41">
         <v>15</v>
       </c>
-      <c r="B17" s="36"/>
+      <c r="B17" s="36" t="s">
+        <v>304</v>
+      </c>
       <c r="C17" s="26"/>
     </row>
     <row r="18" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A18" s="41"/>
-      <c r="B18" s="36"/>
+      <c r="B18" s="36" t="s">
+        <v>305</v>
+      </c>
       <c r="C18" s="26"/>
     </row>
     <row r="19" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A19" s="41"/>
-      <c r="B19" s="36"/>
+      <c r="B19" s="36" t="s">
+        <v>306</v>
+      </c>
       <c r="C19" s="26"/>
     </row>
     <row r="20" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
@@ -6494,7 +6612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -6750,7 +6868,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6782,42 +6900,54 @@
       <c r="A3" s="41">
         <v>1</v>
       </c>
-      <c r="B3" s="36"/>
+      <c r="B3" s="36" t="s">
+        <v>297</v>
+      </c>
       <c r="C3" s="26"/>
     </row>
     <row r="4" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A4" s="41">
         <v>2</v>
       </c>
-      <c r="B4" s="36"/>
+      <c r="B4" s="36" t="s">
+        <v>298</v>
+      </c>
       <c r="C4" s="26"/>
     </row>
-    <row r="5" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="78" x14ac:dyDescent="0.25">
       <c r="A5" s="41">
         <v>3</v>
       </c>
-      <c r="B5" s="36"/>
+      <c r="B5" s="36" t="s">
+        <v>299</v>
+      </c>
       <c r="C5" s="26"/>
     </row>
-    <row r="6" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="78" x14ac:dyDescent="0.25">
       <c r="A6" s="41">
         <v>4</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="36" t="s">
+        <v>300</v>
+      </c>
       <c r="C6" s="26"/>
     </row>
-    <row r="7" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A7" s="41">
         <v>5</v>
       </c>
-      <c r="B7" s="36"/>
+      <c r="B7" s="36" t="s">
+        <v>301</v>
+      </c>
       <c r="C7" s="26"/>
     </row>
     <row r="8" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A8" s="41">
         <v>6</v>
       </c>
-      <c r="B8" s="36"/>
+      <c r="B8" s="36" t="s">
+        <v>302</v>
+      </c>
       <c r="C8" s="26"/>
     </row>
     <row r="9" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
@@ -6972,6 +7102,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>